<commit_message>
add size of cash
</commit_message>
<xml_diff>
--- a/Trainy-project/Results.xlsx
+++ b/Trainy-project/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A498E-8795-4C70-A0C9-05AEAF64BD55}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7120D05C-8407-40E3-ADB6-B1AB7386D91E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VS Compiler" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="9">
   <si>
     <t>Sequence, sec</t>
   </si>
@@ -51,6 +51,9 @@
   <si>
     <t>Acceleration</t>
   </si>
+  <si>
+    <t>Cash level3 = 8MB</t>
+  </si>
 </sst>
 </file>
 
@@ -65,12 +68,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -94,6 +103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -5241,8 +5251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5345,15 +5355,15 @@
         <v>1000</v>
       </c>
       <c r="K3">
-        <f>C3/F3</f>
+        <f t="shared" ref="K3:K11" si="0">C3/F3</f>
         <v>1.0154855571124997</v>
       </c>
       <c r="L3">
-        <f>D3/G3</f>
+        <f t="shared" ref="L3:L11" si="1">D3/G3</f>
         <v>0.98099220380823615</v>
       </c>
       <c r="M3">
-        <f>E3/H3</f>
+        <f t="shared" ref="M3:M11" si="2">E3/H3</f>
         <v>1.0376622459847091</v>
       </c>
     </row>
@@ -5386,15 +5396,15 @@
         <v>1500</v>
       </c>
       <c r="K4">
-        <f>C4/F4</f>
+        <f t="shared" si="0"/>
         <v>1.146560982439728</v>
       </c>
       <c r="L4">
-        <f>D4/G4</f>
+        <f t="shared" si="1"/>
         <v>1.0088307053226853</v>
       </c>
       <c r="M4">
-        <f>E4/H4</f>
+        <f t="shared" si="2"/>
         <v>0.99121215202733515</v>
       </c>
     </row>
@@ -5427,15 +5437,15 @@
         <v>2000</v>
       </c>
       <c r="K5">
-        <f>C5/F5</f>
+        <f t="shared" si="0"/>
         <v>0.99683446862812475</v>
       </c>
       <c r="L5">
-        <f>D5/G5</f>
+        <f t="shared" si="1"/>
         <v>0.98678984754548815</v>
       </c>
       <c r="M5">
-        <f>E5/H5</f>
+        <f t="shared" si="2"/>
         <v>0.9763153214877579</v>
       </c>
     </row>
@@ -5468,15 +5478,15 @@
         <v>2500</v>
       </c>
       <c r="K6">
-        <f>C6/F6</f>
+        <f t="shared" si="0"/>
         <v>1.1008884829961243</v>
       </c>
       <c r="L6">
-        <f>D6/G6</f>
+        <f t="shared" si="1"/>
         <v>1.0185962072704293</v>
       </c>
       <c r="M6">
-        <f>E6/H6</f>
+        <f t="shared" si="2"/>
         <v>0.93765116365772638</v>
       </c>
     </row>
@@ -5509,15 +5519,15 @@
         <v>3000</v>
       </c>
       <c r="K7">
-        <f>C7/F7</f>
+        <f t="shared" si="0"/>
         <v>1.0303672016000591</v>
       </c>
       <c r="L7">
-        <f>D7/G7</f>
+        <f t="shared" si="1"/>
         <v>1.0023770179571978</v>
       </c>
       <c r="M7">
-        <f>E7/H7</f>
+        <f t="shared" si="2"/>
         <v>1.1077205546451432</v>
       </c>
     </row>
@@ -5550,15 +5560,15 @@
         <v>3500</v>
       </c>
       <c r="K8">
-        <f>C8/F8</f>
+        <f t="shared" si="0"/>
         <v>0.93333983540028542</v>
       </c>
       <c r="L8">
-        <f>D8/G8</f>
+        <f t="shared" si="1"/>
         <v>1.3577089501023025</v>
       </c>
       <c r="M8">
-        <f>E8/H8</f>
+        <f t="shared" si="2"/>
         <v>0.99152441044649564</v>
       </c>
     </row>
@@ -5591,15 +5601,15 @@
         <v>4000</v>
       </c>
       <c r="K9">
-        <f>C9/F9</f>
+        <f t="shared" si="0"/>
         <v>1.0085640788831427</v>
       </c>
       <c r="L9">
-        <f>D9/G9</f>
+        <f t="shared" si="1"/>
         <v>1.0436981929019571</v>
       </c>
       <c r="M9">
-        <f>E9/H9</f>
+        <f t="shared" si="2"/>
         <v>1.0831644529001097</v>
       </c>
     </row>
@@ -5632,15 +5642,15 @@
         <v>4500</v>
       </c>
       <c r="K10">
-        <f>C10/F10</f>
+        <f t="shared" si="0"/>
         <v>0.99500804638773821</v>
       </c>
       <c r="L10">
-        <f>D10/G10</f>
+        <f t="shared" si="1"/>
         <v>0.98304501994092641</v>
       </c>
       <c r="M10">
-        <f>E10/H10</f>
+        <f t="shared" si="2"/>
         <v>0.94672058313524921</v>
       </c>
     </row>
@@ -5673,15 +5683,15 @@
         <v>5000</v>
       </c>
       <c r="K11">
-        <f>C11/F11</f>
+        <f t="shared" si="0"/>
         <v>0.85699764588497573</v>
       </c>
       <c r="L11">
-        <f>D11/G11</f>
+        <f t="shared" si="1"/>
         <v>1.0692022903574077</v>
       </c>
       <c r="M11">
-        <f>E11/H11</f>
+        <f t="shared" si="2"/>
         <v>1.07845280751409</v>
       </c>
     </row>
@@ -5694,6 +5704,9 @@
       </c>
       <c r="D15" t="s">
         <v>6</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -5829,7 +5842,8 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5837,7 +5851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F62617-1192-4ADD-A79F-C9AEE7956519}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>

</xml_diff>